<commit_message>
Se hacen cambios para la automatizacion CambioPrePos
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="66">
   <si>
     <t>MSIDN</t>
   </si>
@@ -199,6 +199,30 @@
   </si>
   <si>
     <t>http://10.69.60.77:8180/tigo-pos-web/wap/windex.wml</t>
+  </si>
+  <si>
+    <t>732111324707274</t>
+  </si>
+  <si>
+    <t>3043208091</t>
+  </si>
+  <si>
+    <t>3043209773</t>
+  </si>
+  <si>
+    <t>732111324707275</t>
+  </si>
+  <si>
+    <t>732111324707276</t>
+  </si>
+  <si>
+    <t>3043209819</t>
+  </si>
+  <si>
+    <t>3043209863</t>
+  </si>
+  <si>
+    <t>732111324707277</t>
   </si>
 </sst>
 </file>
@@ -598,7 +622,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
@@ -755,10 +779,10 @@
         <v>56</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -769,10 +793,10 @@
         <v>52</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -783,10 +807,10 @@
         <v>53</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>27</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -797,10 +821,10 @@
         <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -811,10 +835,10 @@
         <v>55</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nuevos casos de uso para sanity semilla 4 portIn pospago
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="81">
   <si>
     <t>MSIDN</t>
   </si>
@@ -183,21 +183,6 @@
     <t>SIEBEL02</t>
   </si>
   <si>
-    <t>874513783</t>
-  </si>
-  <si>
-    <t>680974538</t>
-  </si>
-  <si>
-    <t>1016141153</t>
-  </si>
-  <si>
-    <t>499757452</t>
-  </si>
-  <si>
-    <t>624917673</t>
-  </si>
-  <si>
     <t>http://10.69.60.77:8180/tigo-pos-web/wap/windex.wml</t>
   </si>
   <si>
@@ -219,10 +204,70 @@
     <t>3043209819</t>
   </si>
   <si>
-    <t>3043209863</t>
-  </si>
-  <si>
     <t>732111324707277</t>
+  </si>
+  <si>
+    <t>501506363</t>
+  </si>
+  <si>
+    <t>933727137</t>
+  </si>
+  <si>
+    <t>333489166</t>
+  </si>
+  <si>
+    <t>725586919</t>
+  </si>
+  <si>
+    <t>25620076</t>
+  </si>
+  <si>
+    <t>3043209868</t>
+  </si>
+  <si>
+    <t>3045981684</t>
+  </si>
+  <si>
+    <t>732111193278813</t>
+  </si>
+  <si>
+    <t>3045981670</t>
+  </si>
+  <si>
+    <t>732111193278811</t>
+  </si>
+  <si>
+    <t>msisdn</t>
+  </si>
+  <si>
+    <t>msi</t>
+  </si>
+  <si>
+    <t>nip</t>
+  </si>
+  <si>
+    <t>81684</t>
+  </si>
+  <si>
+    <t>81670</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>1061520830</t>
+  </si>
+  <si>
+    <t>111295346</t>
+  </si>
+  <si>
+    <t>portId</t>
+  </si>
+  <si>
+    <t>00002201108240181684</t>
+  </si>
+  <si>
+    <t>00002201108240181670</t>
   </si>
 </sst>
 </file>
@@ -619,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
@@ -631,11 +676,13 @@
     <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="52.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.453125" style="1"/>
+    <col min="5" max="5" width="22.08984375" style="1" customWidth="1"/>
+    <col min="6" max="8" width="11.453125" style="1"/>
+    <col min="9" max="9" width="22.36328125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -661,7 +708,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -669,7 +716,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
@@ -687,7 +734,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -701,7 +748,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -715,7 +762,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
@@ -729,7 +776,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
@@ -743,7 +790,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
@@ -757,7 +804,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
@@ -770,75 +817,120 @@
       <c r="D8" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="E8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>53</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>56</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se crea las clases PortabilityPrepaidActions y PortabilityPrepaidPage, con la correcion de metodos de la clase DatabasePortInActions y se crea el el execute.feature el escenario para la portabilidad prepago.
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla4\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23760EA-5EF1-4709-B8F6-19DE95CBD7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 4" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="82">
   <si>
     <t>MSIDN</t>
   </si>
@@ -268,12 +269,15 @@
   </si>
   <si>
     <t>00002201108240181670</t>
+  </si>
+  <si>
+    <t>URL Portabilidad SoapUI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -663,23 +667,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.08984375" style="1" customWidth="1"/>
-    <col min="6" max="8" width="11.453125" style="1"/>
-    <col min="9" max="9" width="22.36328125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.453125" style="1"/>
+    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="1" customWidth="1"/>
+    <col min="6" max="8" width="11.42578125" style="1"/>
+    <col min="9" max="9" width="22.42578125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -707,6 +711,9 @@
       <c r="H1" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
@@ -935,11 +942,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
-    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -947,20 +954,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1796875" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" customWidth="1"/>
-    <col min="3" max="3" width="24.6328125" customWidth="1"/>
-    <col min="4" max="4" width="31.1796875" customWidth="1"/>
-    <col min="5" max="5" width="30.81640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
@@ -1171,11 +1178,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
-    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
sanity semilla 4 portIn pospago
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla4\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23760EA-5EF1-4709-B8F6-19DE95CBD7B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 4" sheetId="1" r:id="rId1"/>
@@ -277,7 +276,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -667,23 +666,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" style="1" customWidth="1"/>
-    <col min="6" max="8" width="11.42578125" style="1"/>
-    <col min="9" max="9" width="22.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="17.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.90625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="11.453125" style="1"/>
+    <col min="9" max="9" width="22.453125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -942,11 +942,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -954,20 +954,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.1796875" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" customWidth="1"/>
+    <col min="4" max="4" width="31.1796875" customWidth="1"/>
+    <col min="5" max="5" width="30.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
@@ -1178,11 +1178,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="B2" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se hace depuracion de metodos para la PortabilityPrepaidActions
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla4\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF7E0D8-DC25-4E00-8CF7-D9AEFFC6CC04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 4" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="83">
   <si>
     <t>MSIDN</t>
   </si>
@@ -271,12 +272,15 @@
   </si>
   <si>
     <t>URL Portabilidad SoapUI</t>
+  </si>
+  <si>
+    <t>http://10.69.60.76:8080/PortabilidadServiceEAR-HPNPCommunicationsDelegateEJB/NPCRMWSImpl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -336,7 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -350,6 +354,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -666,24 +673,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.1796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1796875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.90625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="11.453125" style="1"/>
-    <col min="9" max="9" width="22.453125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.453125" style="1"/>
+    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="1" customWidth="1"/>
+    <col min="6" max="8" width="11.42578125" style="1"/>
+    <col min="9" max="9" width="22.42578125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -740,6 +746,9 @@
       <c r="H2" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="I2" s="7" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
@@ -942,32 +951,33 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
-    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="I2" r:id="rId6" xr:uid="{235730A1-C277-40DE-A808-35BD3C4AF782}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.1796875" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" customWidth="1"/>
-    <col min="3" max="3" width="24.54296875" customWidth="1"/>
-    <col min="4" max="4" width="31.1796875" customWidth="1"/>
-    <col min="5" max="5" width="30.81640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
@@ -1178,11 +1188,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="B2" r:id="rId4"/>
-    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ejecucion de ssh para portIn
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="88">
   <si>
     <t>MSIDN</t>
   </si>
@@ -274,13 +274,28 @@
   </si>
   <si>
     <t>3045984642</t>
+  </si>
+  <si>
+    <t>host ssh</t>
+  </si>
+  <si>
+    <t>usuario ssh</t>
+  </si>
+  <si>
+    <t>contraseña ssh</t>
+  </si>
+  <si>
+    <t>consulta_log</t>
+  </si>
+  <si>
+    <t>10.69.60.76</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,6 +332,21 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -339,7 +369,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -358,6 +388,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -675,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
@@ -776,6 +810,15 @@
       <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="E4" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
@@ -789,6 +832,15 @@
       </c>
       <c r="D5" s="5" t="s">
         <v>17</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:9">

</xml_diff>

<commit_message>
Ejecucion de ssh exitosa
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -709,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5"/>
@@ -720,7 +720,9 @@
     <col min="3" max="3" width="18.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.1796875" style="1" customWidth="1"/>
     <col min="5" max="5" width="22.1796875" style="1" customWidth="1"/>
-    <col min="6" max="8" width="11.453125" style="1"/>
+    <col min="6" max="6" width="17.1796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.36328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" style="1"/>
     <col min="9" max="9" width="22.453125" style="1" customWidth="1"/>
     <col min="10" max="16384" width="11.453125" style="1"/>
   </cols>

</xml_diff>

<commit_message>
se agregan un scroll y tiempos de espera para la clase ControlActivationActions, se instala localmente el winwap y se ajusta la ruta en el data.excel
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla4\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F967E6F5-7408-418D-A1B1-728A9E69926A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4A9CAC-2526-45BC-B180-0627B15BC0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="18775" windowHeight="10067" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 4" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="79">
   <si>
     <t>MSIDN</t>
   </si>
@@ -260,6 +260,9 @@
   </si>
   <si>
     <t>732111324707278</t>
+  </si>
+  <si>
+    <t>src/test/resources/winwap/WinWAP for Windows 4.2/WinWAP4.exe</t>
   </si>
 </sst>
 </file>
@@ -684,16 +687,16 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="14.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" style="1" customWidth="1"/>
-    <col min="6" max="8" width="11.42578125" style="1"/>
-    <col min="9" max="9" width="22.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="17.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.125" style="1" customWidth="1"/>
+    <col min="6" max="8" width="11.375" style="1"/>
+    <col min="9" max="9" width="22.375" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1003,17 +1006,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.125" customWidth="1"/>
+    <col min="2" max="2" width="22.125" customWidth="1"/>
+    <col min="3" max="3" width="24.625" customWidth="1"/>
+    <col min="4" max="4" width="31.125" customWidth="1"/>
+    <col min="5" max="5" width="30.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1">
@@ -1068,7 +1071,7 @@
         <v>31</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
se elimina el wimwap
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla4\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4A9CAC-2526-45BC-B180-0627B15BC0BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B50B7D-3800-4C50-AEAF-0D2F97428291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="18775" windowHeight="10067" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="78">
   <si>
     <t>MSIDN</t>
   </si>
@@ -260,9 +260,6 @@
   </si>
   <si>
     <t>732111324707278</t>
-  </si>
-  <si>
-    <t>src/test/resources/winwap/WinWAP for Windows 4.2/WinWAP4.exe</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1004,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3"/>
@@ -1071,7 +1068,7 @@
         <v>31</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
se agregan metodos y clases para la legalizacion del pedido
</commit_message>
<xml_diff>
--- a/src/test/resources/config_data/data.xlsx
+++ b/src/test/resources/config_data/data.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla4\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B50B7D-3800-4C50-AEAF-0D2F97428291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D917CC45-8C31-45B5-9956-A96ADFDB2CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="18775" windowHeight="10067" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Semilla 4" sheetId="1" r:id="rId1"/>
-    <sheet name="Semilla 3" sheetId="2" r:id="rId2"/>
+    <sheet name="Semilla 3" sheetId="2" r:id="rId1"/>
+    <sheet name="Semilla 6" sheetId="4" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="78">
   <si>
     <t>MSIDN</t>
   </si>
@@ -46,12 +46,6 @@
     <t>URL GATEWAY MG</t>
   </si>
   <si>
-    <t>http://10.69.60.77:8180/tigo-pos-web/</t>
-  </si>
-  <si>
-    <t>http://10.69.60.85:8280/portal/login?initialURI=%2Fportal%2FCRMPortal</t>
-  </si>
-  <si>
     <t>http://10.65.45.12:9001/gatewaycbs/BcServicesInt</t>
   </si>
   <si>
@@ -64,18 +58,12 @@
     <t>password</t>
   </si>
   <si>
-    <t>10.69.60.89</t>
-  </si>
-  <si>
     <t>DEV11G</t>
   </si>
   <si>
     <t>ACTIVATOR</t>
   </si>
   <si>
-    <t>10.69.60.88</t>
-  </si>
-  <si>
     <t>desepos</t>
   </si>
   <si>
@@ -91,9 +79,6 @@
     <t>10.65.32.74</t>
   </si>
   <si>
-    <t>siebel04</t>
-  </si>
-  <si>
     <t>siebel</t>
   </si>
   <si>
@@ -136,21 +121,9 @@
     <t>http://10.69.60.106:8180/tigo-pos-web/index.jsp</t>
   </si>
   <si>
-    <t>10.69.60.103</t>
-  </si>
-  <si>
-    <t>10.69.60.102</t>
-  </si>
-  <si>
-    <t>10.65.32.76</t>
-  </si>
-  <si>
     <t>SIEBEL02</t>
   </si>
   <si>
-    <t>http://10.69.60.77:8180/tigo-pos-web/wap/windex.wml</t>
-  </si>
-  <si>
     <t>732111324707274</t>
   </si>
   <si>
@@ -169,21 +142,6 @@
     <t>3043209819</t>
   </si>
   <si>
-    <t>501506363</t>
-  </si>
-  <si>
-    <t>933727137</t>
-  </si>
-  <si>
-    <t>333489166</t>
-  </si>
-  <si>
-    <t>725586919</t>
-  </si>
-  <si>
-    <t>25620076</t>
-  </si>
-  <si>
     <t>3043209868</t>
   </si>
   <si>
@@ -250,16 +208,58 @@
     <t>consulta_log</t>
   </si>
   <si>
-    <t>10.69.60.76</t>
-  </si>
-  <si>
-    <t>3043209863</t>
+    <t>10.69.60.87</t>
+  </si>
+  <si>
+    <t>dev11g</t>
+  </si>
+  <si>
+    <t>10.69.60.86</t>
+  </si>
+  <si>
+    <t>SIEBEL03</t>
+  </si>
+  <si>
+    <t>10.69.60.105</t>
+  </si>
+  <si>
+    <t>566984435</t>
+  </si>
+  <si>
+    <t>887082715</t>
+  </si>
+  <si>
+    <t>613706262</t>
+  </si>
+  <si>
+    <t>621218573</t>
+  </si>
+  <si>
+    <t>732111324707278</t>
   </si>
   <si>
     <t xml:space="preserve">732111324707277 </t>
   </si>
   <si>
-    <t>732111324707278</t>
+    <t>http://10.69.60.57:8180/tigo-pos-web/index.jsp</t>
+  </si>
+  <si>
+    <t>http://10.69.60.61:8280/portal/login?initialURI=%2Fportal%2FCRMPortal%2FVenta</t>
+  </si>
+  <si>
+    <t>http://10.69.60.57:8180/tigo-pos-web/wap/windex.wml</t>
+  </si>
+  <si>
+    <t>10.69.60.63</t>
+  </si>
+  <si>
+    <t>http://10.69.60.56:8080/PortabilidadServiceEAR-HPNPCommunicationsDelegateEJB/NPCRMWSImpl</t>
+  </si>
+  <si>
+    <t>10.69.60.62</t>
+  </si>
+  <si>
+    <t>10.69.60.56</t>
   </si>
 </sst>
 </file>
@@ -677,343 +677,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="14.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.125" style="1" customWidth="1"/>
-    <col min="6" max="8" width="11.375" style="1"/>
-    <col min="9" max="9" width="22.375" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.375" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="I2" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I24"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3"/>
-  <cols>
-    <col min="1" max="1" width="26.125" customWidth="1"/>
-    <col min="2" max="2" width="22.125" customWidth="1"/>
-    <col min="3" max="3" width="24.625" customWidth="1"/>
-    <col min="4" max="4" width="31.125" customWidth="1"/>
-    <col min="5" max="5" width="30.875" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1">
@@ -1033,337 +710,277 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1">
       <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="1" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>36</v>
+        <v>74</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1">
       <c r="A5" s="5" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1">
       <c r="A7" s="5" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="1" customFormat="1">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="I9" s="1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="1" customFormat="1">
       <c r="A10" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="I10" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="1" customFormat="1">
       <c r="A11" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="1" customFormat="1">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3043209863</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1375,5 +992,325 @@
     <hyperlink ref="I2" r:id="rId6" xr:uid="{F95E11DB-0174-40E5-880B-10A9CAE9721D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D188C588-523E-4AEF-A066-FA5DCECDB773}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1">
+      <c r="A4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1">
+      <c r="A5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1">
+      <c r="A6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="1" customFormat="1">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="1" customFormat="1">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="1" customFormat="1">
+      <c r="A12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="1" customFormat="1">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="1">
+        <v>3043209863</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{AE7E7D5F-3451-46BE-B31F-CDFFAB87FAF3}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{B07F7B86-3047-4A07-9BE1-E38D783D7D3F}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{7EF9C36A-A817-482C-949F-0558C7D8177E}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{FE3DDCF9-FF16-45B7-8B3A-8ECE870141C5}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{C8CB93F0-4784-4DEB-AE0D-6AF2969E9824}"/>
+    <hyperlink ref="I2" r:id="rId6" xr:uid="{FB4AC1A2-9E3E-4783-AB76-1C415E1BF0B2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>